<commit_message>
cambios separadores de miles
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
-  <si>
-    <t>ARCELORMITTAL</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+  <si>
+    <t>DEACERO</t>
   </si>
   <si>
     <t>Folio</t>
@@ -46,27 +46,24 @@
     <t>Peso Recibido en Kg</t>
   </si>
   <si>
-    <t>RMH-0001</t>
-  </si>
-  <si>
-    <t>TALLER DE SMC</t>
-  </si>
-  <si>
-    <t>Varilla #9</t>
+    <t>RMH-0004</t>
+  </si>
+  <si>
+    <t>TALLER DE COREMAN</t>
   </si>
   <si>
     <t>Varilla #5</t>
   </si>
   <si>
-    <t>RMH-0002</t>
-  </si>
-  <si>
-    <t>Varilla #11</t>
+    <t>21/06/2016</t>
   </si>
   <si>
     <t>Varilla #7</t>
   </si>
   <si>
+    <t>Varilla #10</t>
+  </si>
+  <si>
     <t>Fecha de Envio</t>
   </si>
   <si>
@@ -80,24 +77,6 @@
   </si>
   <si>
     <t>Peso Asignado en Kg</t>
-  </si>
-  <si>
-    <t>SMH-0001</t>
-  </si>
-  <si>
-    <t>Viaducto 1A</t>
-  </si>
-  <si>
-    <t>1A-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Capitel I</t>
-  </si>
-  <si>
-    <t>SMH-0002</t>
-  </si>
-  <si>
-    <t>1A-2</t>
   </si>
   <si>
     <t>Peso Total en Kg</t>
@@ -475,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -535,25 +514,25 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>123</v>
+        <v>543</v>
       </c>
       <c r="D3">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3">
-        <v>330.78</v>
+        <v>964.57</v>
       </c>
       <c r="G3">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>42542</v>
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
       <c r="I3">
-        <v>40500</v>
+        <v>67070</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -564,25 +543,25 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>123</v>
+        <v>543</v>
       </c>
       <c r="D4">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>535.87</v>
+        <v>144.9</v>
       </c>
       <c r="G4">
         <v>12</v>
       </c>
-      <c r="H4">
-        <v>42542</v>
+      <c r="H4" t="s">
+        <v>13</v>
       </c>
       <c r="I4">
-        <v>40500</v>
+        <v>67070</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -593,261 +572,76 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>123</v>
+        <v>543</v>
       </c>
       <c r="D5">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>562.66</v>
+        <v>626.57</v>
       </c>
       <c r="G5">
         <v>12</v>
       </c>
-      <c r="H5">
-        <v>42542</v>
+      <c r="H5" t="s">
+        <v>13</v>
       </c>
       <c r="I5">
-        <v>40500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>150</v>
-      </c>
-      <c r="D6">
-        <v>123</v>
-      </c>
-      <c r="E6" t="s">
+        <v>67070</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
-        <v>517.05</v>
-      </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
-      <c r="H6">
-        <v>42542</v>
-      </c>
-      <c r="I6">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>150</v>
-      </c>
-      <c r="D7">
-        <v>123</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>144.9</v>
-      </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>42542</v>
-      </c>
-      <c r="I7">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8">
-        <v>123</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>803.81</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>42542</v>
-      </c>
-      <c r="I8">
-        <v>67000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>46700</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17">
-        <v>25000</v>
+      <c r="B10">
+        <v>46770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>